<commit_message>
Cambios generales con EDA
</commit_message>
<xml_diff>
--- a/outputs/reporte_inversion.xlsx
+++ b/outputs/reporte_inversion.xlsx
@@ -11,6 +11,8 @@
     <sheet name="Señal" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Operacion" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Métricas" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Métricas Modelo" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Historico Métricas" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20,8 +22,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -61,12 +63,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,45 +466,703 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>45832.30208333334</v>
+      <c r="A2" s="3" t="n">
+        <v>45887.88194444445</v>
       </c>
       <c r="B2" t="n">
-        <v>1.161527265789267</v>
+        <v>1.166111450612579</v>
       </c>
       <c r="C2" t="n">
-        <v>1.160193370965258</v>
+        <v>1.165350930994731</v>
       </c>
       <c r="D2" t="n">
-        <v>1.162911920643674</v>
+        <v>1.166910302437872</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45832.30555555555</v>
+      <c r="A3" s="3" t="n">
+        <v>45887.88541666666</v>
       </c>
       <c r="B3" t="n">
-        <v>1.16155604534777</v>
+        <v>1.166099581043685</v>
       </c>
       <c r="C3" t="n">
-        <v>1.160217160811391</v>
+        <v>1.165307543281495</v>
       </c>
       <c r="D3" t="n">
-        <v>1.163032192821169</v>
+        <v>1.166802271836846</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45832.30902777778</v>
+      <c r="A4" s="3" t="n">
+        <v>45887.88888888889</v>
       </c>
       <c r="B4" t="n">
-        <v>1.161584176805446</v>
+        <v>1.16608804143314</v>
       </c>
       <c r="C4" t="n">
-        <v>1.160149603684732</v>
+        <v>1.165339004623223</v>
       </c>
       <c r="D4" t="n">
-        <v>1.163028983408583</v>
+        <v>1.166868248762571</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>45887.89236111111</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.166076834619953</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.165356814455954</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.166905377719784</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>45887.89583333334</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.166065963421745</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.165276189783327</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.166812514510006</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>45887.89930555555</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.166055430635064</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.165335603503416</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.16682175584383</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>45887.90277777778</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.166045239034739</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.165202865591963</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.16676276024188</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>45887.90625</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.16603539137391</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.165261125826832</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.166850723266262</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>45887.90972222222</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.166025890383744</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.165179730682044</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.166789757102707</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>45887.91319444445</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.166016738773116</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.165213565098156</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.166791884254839</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>45887.91666666666</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1.166007939228512</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.165194175391721</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.166823612751219</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>45887.92013888889</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1.165999494413606</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.165190793174172</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.166745956365706</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>45887.92361111111</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.165991406969473</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1.165191450419284</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.166793432764846</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>45887.92708333334</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1.165983679513777</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1.165204600233869</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1.166768745774443</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>45887.93055555555</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1.165976314641037</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.165184889192143</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.166835483904235</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>45887.93402777778</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1.165969314922212</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.165111423829811</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.166784320996739</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>45887.9375</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1.165962682904576</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.165133454349764</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.166776984625084</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>45887.94097222222</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1.16595642111143</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.165103506776176</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.166761452020904</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>45887.94444444445</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1.165950532041855</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1.16508956576229</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.166827658082954</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>45887.94791666666</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1.16594501817066</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.165134891620164</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.166764300976614</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>45887.95138888889</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1.165939881948125</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1.165075274957356</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.166713859977198</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>45887.95486111111</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1.165935125799757</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.165072207330531</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.166749590116216</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>45887.95833333334</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1.16593075212605</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.165063776785303</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.166761075960662</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="n">
+        <v>45887.96180555555</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.165926763302414</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1.165032964552154</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.166842506660156</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="n">
+        <v>45887.96527777778</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.16592316167893</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1.164991416998541</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.166769823310522</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="n">
+        <v>45887.96875</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1.165919949580151</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1.165007331219358</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.166805737294266</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="n">
+        <v>45887.97222222222</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.165917129304881</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1.164995937140219</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.166817537518765</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="n">
+        <v>45887.97569444445</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.165914703126042</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1.164960843052714</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.166801188822903</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="n">
+        <v>45887.97916666666</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.16591267329054</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1.165004841869653</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.166769730301765</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="n">
+        <v>45887.98263888889</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.165911042018876</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1.165024747079715</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.166811529687462</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="n">
+        <v>45887.98611111111</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1.165909811505237</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1.164968876784187</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.166803618590016</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="n">
+        <v>45887.98958333334</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1.165908983917058</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1.165039228090216</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1.166841453150235</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="n">
+        <v>45887.99305555555</v>
+      </c>
+      <c r="B34" t="n">
+        <v>1.165908561395109</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1.16496835222641</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.166817273813524</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="n">
+        <v>45887.99652777778</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1.165908546053113</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1.165007433633424</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1.16680502193797</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="n">
+        <v>45888</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1.165908939977675</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1.165036813220352</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.166836513146237</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="n">
+        <v>45888.00347222222</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1.165909745228063</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1.164962394195723</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.166826117850115</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="n">
+        <v>45888.00694444445</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1.1659109638361</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1.16491321162177</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1.16681880303222</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="n">
+        <v>45888.01041666666</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1.165912597805971</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1.164885420777068</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1.166853407201025</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="n">
+        <v>45888.01388888889</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1.165914649114028</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1.164945827383602</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1.16685508834651</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="n">
+        <v>45888.01736111111</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1.165917119708739</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1.164908754589213</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1.166919034746204</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="n">
+        <v>45888.02083333334</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1.165920011510298</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1.164844817617458</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1.166923337335377</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="n">
+        <v>45888.02430555555</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1.16592332641085</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1.164817507028278</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1.166822013325274</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="n">
+        <v>45888.02777777778</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1.165927066273962</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1.164868449522612</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1.166955949589592</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="n">
+        <v>45888.03125</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1.165931232934661</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1.164895602259762</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1.1669055651678</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="n">
+        <v>45888.03472222222</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1.165935828199314</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1.164761154757448</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1.166943782601546</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="n">
+        <v>45888.03819444445</v>
+      </c>
+      <c r="B47" t="n">
+        <v>1.165940853845377</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1.164867142812343</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1.166949821656841</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="n">
+        <v>45888.04166666666</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.165946311621344</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1.164859491295605</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1.166969918332884</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="n">
+        <v>45888.04513888889</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1.165952203246485</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1.164887727412576</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1.167025521093946</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="n">
+        <v>45888.04861111111</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.165958530410946</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1.164922668541363</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1.167026096808181</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="n">
+        <v>45888.05208333334</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1.165965294775256</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1.164777105662496</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1.167042912342661</v>
       </c>
     </row>
   </sheetData>
@@ -555,10 +1216,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0002</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>45831.96540603937</v>
+        <v>0.0005</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>45887.54703189815</v>
       </c>
     </row>
   </sheetData>
@@ -612,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.16031</v>
+        <v>1.1665</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -668,10 +1329,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.8e-05</v>
+        <v>7e-06</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0024</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -682,7 +1343,273 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0002</v>
+        <v>0.0005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Simbolo</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Timeframe</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Modelo</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Pasos_pred</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MAE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>RMSE</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>MAPE_%</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>R2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Sortino</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy_direccional</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Horizonte_dias</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Horizonte_horas_totales</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>45887.54705987268</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>M5</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>prophet</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>50</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0003469403831574303</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0004339600357957925</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.02973148080781424</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.4608994126733642</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.4013161612794071</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4.083333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Simbolo</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Timeframe</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Modelo</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Pasos_pred</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MAE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>RMSE</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>MAPE_%</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>R2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Sortino</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy_direccional</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Horizonte_dias</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Horizonte_horas_totales</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>45887.5470598722</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>M5</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>prophet</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>50</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0003469403831574303</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0004339600357957925</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.02973148080781424</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.4608994126733642</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.4013161612794071</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4.083333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualiza el repositorio con el análisis exploratorio
</commit_message>
<xml_diff>
--- a/outputs/reporte_inversion.xlsx
+++ b/outputs/reporte_inversion.xlsx
@@ -11,8 +11,6 @@
     <sheet name="Señal" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Operacion" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Métricas" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Métricas Modelo" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Historico Métricas" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -22,8 +20,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -63,13 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -435,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,703 +463,1403 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="n">
-        <v>45887.88194444445</v>
+      <c r="A2" s="2" t="n">
+        <v>45891.26388888889</v>
       </c>
       <c r="B2" t="n">
-        <v>1.166111450612579</v>
+        <v>1.160686037850352</v>
       </c>
       <c r="C2" t="n">
-        <v>1.165350930994731</v>
+        <v>1.159902374365517</v>
       </c>
       <c r="D2" t="n">
-        <v>1.166910302437872</v>
+        <v>1.16147909320641</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n">
-        <v>45887.88541666666</v>
+      <c r="A3" s="2" t="n">
+        <v>45891.26736111111</v>
       </c>
       <c r="B3" t="n">
-        <v>1.166099581043685</v>
+        <v>1.160691186448152</v>
       </c>
       <c r="C3" t="n">
-        <v>1.165307543281495</v>
+        <v>1.159956135049903</v>
       </c>
       <c r="D3" t="n">
-        <v>1.166802271836846</v>
+        <v>1.161455192562638</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>45887.88888888889</v>
+      <c r="A4" s="2" t="n">
+        <v>45891.27083333334</v>
       </c>
       <c r="B4" t="n">
-        <v>1.16608804143314</v>
+        <v>1.160696663852637</v>
       </c>
       <c r="C4" t="n">
-        <v>1.165339004623223</v>
+        <v>1.159912339492364</v>
       </c>
       <c r="D4" t="n">
-        <v>1.166868248762571</v>
+        <v>1.161427191667467</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>45887.89236111111</v>
+      <c r="A5" s="2" t="n">
+        <v>45891.27430555555</v>
       </c>
       <c r="B5" t="n">
-        <v>1.166076834619953</v>
+        <v>1.160702471425232</v>
       </c>
       <c r="C5" t="n">
-        <v>1.165356814455954</v>
+        <v>1.159893077792637</v>
       </c>
       <c r="D5" t="n">
-        <v>1.166905377719784</v>
+        <v>1.161493349102711</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>45887.89583333334</v>
+      <c r="A6" s="2" t="n">
+        <v>45891.27777777778</v>
       </c>
       <c r="B6" t="n">
-        <v>1.166065963421745</v>
+        <v>1.160708610509751</v>
       </c>
       <c r="C6" t="n">
-        <v>1.165276189783327</v>
+        <v>1.15994617999731</v>
       </c>
       <c r="D6" t="n">
-        <v>1.166812514510006</v>
+        <v>1.161457726298092</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n">
-        <v>45887.89930555555</v>
+      <c r="A7" s="2" t="n">
+        <v>45891.28125</v>
       </c>
       <c r="B7" t="n">
-        <v>1.166055430635064</v>
+        <v>1.160715082432181</v>
       </c>
       <c r="C7" t="n">
-        <v>1.165335603503416</v>
+        <v>1.159929118942929</v>
       </c>
       <c r="D7" t="n">
-        <v>1.16682175584383</v>
+        <v>1.161495681362763</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n">
-        <v>45887.90277777778</v>
+      <c r="A8" s="2" t="n">
+        <v>45891.28472222222</v>
       </c>
       <c r="B8" t="n">
-        <v>1.166045239034739</v>
+        <v>1.160721888500633</v>
       </c>
       <c r="C8" t="n">
-        <v>1.165202865591963</v>
+        <v>1.15993274510925</v>
       </c>
       <c r="D8" t="n">
-        <v>1.16676276024188</v>
+        <v>1.161465455118887</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="n">
-        <v>45887.90625</v>
+      <c r="A9" s="2" t="n">
+        <v>45891.28819444445</v>
       </c>
       <c r="B9" t="n">
-        <v>1.16603539137391</v>
+        <v>1.160729030005155</v>
       </c>
       <c r="C9" t="n">
-        <v>1.165261125826832</v>
+        <v>1.159941967673027</v>
       </c>
       <c r="D9" t="n">
-        <v>1.166850723266262</v>
+        <v>1.161473989609445</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n">
-        <v>45887.90972222222</v>
+      <c r="A10" s="2" t="n">
+        <v>45891.29166666666</v>
       </c>
       <c r="B10" t="n">
-        <v>1.166025890383744</v>
+        <v>1.160736508217679</v>
       </c>
       <c r="C10" t="n">
-        <v>1.165179730682044</v>
+        <v>1.159909087539887</v>
       </c>
       <c r="D10" t="n">
-        <v>1.166789757102707</v>
+        <v>1.161559510625047</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n">
-        <v>45887.91319444445</v>
+      <c r="A11" s="2" t="n">
+        <v>45891.29513888889</v>
       </c>
       <c r="B11" t="n">
-        <v>1.166016738773116</v>
+        <v>1.160744324391822</v>
       </c>
       <c r="C11" t="n">
-        <v>1.165213565098156</v>
+        <v>1.159939094527521</v>
       </c>
       <c r="D11" t="n">
-        <v>1.166791884254839</v>
+        <v>1.161493627521016</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n">
-        <v>45887.91666666666</v>
+      <c r="A12" s="2" t="n">
+        <v>45891.29861111111</v>
       </c>
       <c r="B12" t="n">
-        <v>1.166007939228512</v>
+        <v>1.160752479762783</v>
       </c>
       <c r="C12" t="n">
-        <v>1.165194175391721</v>
+        <v>1.160039642365979</v>
       </c>
       <c r="D12" t="n">
-        <v>1.166823612751219</v>
+        <v>1.161532092856027</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="n">
-        <v>45887.92013888889</v>
+      <c r="A13" s="2" t="n">
+        <v>45891.30208333334</v>
       </c>
       <c r="B13" t="n">
-        <v>1.165999494413606</v>
+        <v>1.160760975547316</v>
       </c>
       <c r="C13" t="n">
-        <v>1.165190793174172</v>
+        <v>1.159981064297903</v>
       </c>
       <c r="D13" t="n">
-        <v>1.166745956365706</v>
+        <v>1.161579494327182</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="n">
-        <v>45887.92361111111</v>
+      <c r="A14" s="2" t="n">
+        <v>45891.30555555555</v>
       </c>
       <c r="B14" t="n">
-        <v>1.165991406969473</v>
+        <v>1.160769812943501</v>
       </c>
       <c r="C14" t="n">
-        <v>1.165191450419284</v>
+        <v>1.159947661685135</v>
       </c>
       <c r="D14" t="n">
-        <v>1.166793432764846</v>
+        <v>1.161530445085436</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="n">
-        <v>45887.92708333334</v>
+      <c r="A15" s="2" t="n">
+        <v>45891.30902777778</v>
       </c>
       <c r="B15" t="n">
-        <v>1.165983679513777</v>
+        <v>1.160778993130598</v>
       </c>
       <c r="C15" t="n">
-        <v>1.165204600233869</v>
+        <v>1.160032413643295</v>
       </c>
       <c r="D15" t="n">
-        <v>1.166768745774443</v>
+        <v>1.161519246652119</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="n">
-        <v>45887.93055555555</v>
+      <c r="A16" s="2" t="n">
+        <v>45891.3125</v>
       </c>
       <c r="B16" t="n">
-        <v>1.165976314641037</v>
+        <v>1.160788517269107</v>
       </c>
       <c r="C16" t="n">
-        <v>1.165184889192143</v>
+        <v>1.159963222138748</v>
       </c>
       <c r="D16" t="n">
-        <v>1.166835483904235</v>
+        <v>1.161585432837036</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="n">
-        <v>45887.93402777778</v>
+      <c r="A17" s="2" t="n">
+        <v>45891.31597222222</v>
       </c>
       <c r="B17" t="n">
-        <v>1.165969314922212</v>
+        <v>1.16079838650046</v>
       </c>
       <c r="C17" t="n">
-        <v>1.165111423829811</v>
+        <v>1.160043783237261</v>
       </c>
       <c r="D17" t="n">
-        <v>1.166784320996739</v>
+        <v>1.161639966280182</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="n">
-        <v>45887.9375</v>
+      <c r="A18" s="2" t="n">
+        <v>45891.31944444445</v>
       </c>
       <c r="B18" t="n">
-        <v>1.165962682904576</v>
+        <v>1.160808601947038</v>
       </c>
       <c r="C18" t="n">
-        <v>1.165133454349764</v>
+        <v>1.160035125315819</v>
       </c>
       <c r="D18" t="n">
-        <v>1.166776984625084</v>
+        <v>1.161592381790227</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="n">
-        <v>45887.94097222222</v>
+      <c r="A19" s="2" t="n">
+        <v>45891.32291666666</v>
       </c>
       <c r="B19" t="n">
-        <v>1.16595642111143</v>
+        <v>1.160819164712009</v>
       </c>
       <c r="C19" t="n">
-        <v>1.165103506776176</v>
+        <v>1.159967008990141</v>
       </c>
       <c r="D19" t="n">
-        <v>1.166761452020904</v>
+        <v>1.161598179360815</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="n">
-        <v>45887.94444444445</v>
+      <c r="A20" s="2" t="n">
+        <v>45891.32638888889</v>
       </c>
       <c r="B20" t="n">
-        <v>1.165950532041855</v>
+        <v>1.160830075879208</v>
       </c>
       <c r="C20" t="n">
-        <v>1.16508956576229</v>
+        <v>1.159985797505277</v>
       </c>
       <c r="D20" t="n">
-        <v>1.166827658082954</v>
+        <v>1.161616055094703</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="n">
-        <v>45887.94791666666</v>
+      <c r="A21" s="2" t="n">
+        <v>45891.32986111111</v>
       </c>
       <c r="B21" t="n">
-        <v>1.16594501817066</v>
+        <v>1.16084133651303</v>
       </c>
       <c r="C21" t="n">
-        <v>1.165134891620164</v>
+        <v>1.160022262967845</v>
       </c>
       <c r="D21" t="n">
-        <v>1.166764300976614</v>
+        <v>1.161665184600928</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="n">
-        <v>45887.95138888889</v>
+      <c r="A22" s="2" t="n">
+        <v>45891.33333333334</v>
       </c>
       <c r="B22" t="n">
-        <v>1.165939881948125</v>
+        <v>1.160852947658408</v>
       </c>
       <c r="C22" t="n">
-        <v>1.165075274957356</v>
+        <v>1.160029891206123</v>
       </c>
       <c r="D22" t="n">
-        <v>1.166713859977198</v>
+        <v>1.161627061009151</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="n">
-        <v>45887.95486111111</v>
+      <c r="A23" s="2" t="n">
+        <v>45891.33680555555</v>
       </c>
       <c r="B23" t="n">
-        <v>1.165935125799757</v>
+        <v>1.160864910340571</v>
       </c>
       <c r="C23" t="n">
-        <v>1.165072207330531</v>
+        <v>1.159965772973125</v>
       </c>
       <c r="D23" t="n">
-        <v>1.166749590116216</v>
+        <v>1.161705629890824</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="n">
-        <v>45887.95833333334</v>
+      <c r="A24" s="2" t="n">
+        <v>45891.34027777778</v>
       </c>
       <c r="B24" t="n">
-        <v>1.16593075212605</v>
+        <v>1.160877225565007</v>
       </c>
       <c r="C24" t="n">
-        <v>1.165063776785303</v>
+        <v>1.160032736238673</v>
       </c>
       <c r="D24" t="n">
-        <v>1.166761075960662</v>
+        <v>1.161729840290558</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="n">
-        <v>45887.96180555555</v>
+      <c r="A25" s="2" t="n">
+        <v>45891.34375</v>
       </c>
       <c r="B25" t="n">
-        <v>1.165926763302414</v>
+        <v>1.160889894317427</v>
       </c>
       <c r="C25" t="n">
-        <v>1.165032964552154</v>
+        <v>1.160051207627806</v>
       </c>
       <c r="D25" t="n">
-        <v>1.166842506660156</v>
+        <v>1.161699182431518</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="n">
-        <v>45887.96527777778</v>
+      <c r="A26" s="2" t="n">
+        <v>45891.34722222222</v>
       </c>
       <c r="B26" t="n">
-        <v>1.16592316167893</v>
+        <v>1.160902917563535</v>
       </c>
       <c r="C26" t="n">
-        <v>1.164991416998541</v>
+        <v>1.160020447729198</v>
       </c>
       <c r="D26" t="n">
-        <v>1.166769823310522</v>
+        <v>1.161783744867272</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="n">
-        <v>45887.96875</v>
+      <c r="A27" s="2" t="n">
+        <v>45891.35069444445</v>
       </c>
       <c r="B27" t="n">
-        <v>1.165919949580151</v>
+        <v>1.160916296248989</v>
       </c>
       <c r="C27" t="n">
-        <v>1.165007331219358</v>
+        <v>1.160046996885487</v>
       </c>
       <c r="D27" t="n">
-        <v>1.166805737294266</v>
+        <v>1.161720618395677</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="n">
-        <v>45887.97222222222</v>
+      <c r="A28" s="2" t="n">
+        <v>45891.35416666666</v>
       </c>
       <c r="B28" t="n">
-        <v>1.165917129304881</v>
+        <v>1.160930031299377</v>
       </c>
       <c r="C28" t="n">
-        <v>1.164995937140219</v>
+        <v>1.160090043266801</v>
       </c>
       <c r="D28" t="n">
-        <v>1.166817537518765</v>
+        <v>1.161748404860946</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="n">
-        <v>45887.97569444445</v>
+      <c r="A29" s="2" t="n">
+        <v>45891.35763888889</v>
       </c>
       <c r="B29" t="n">
-        <v>1.165914703126042</v>
+        <v>1.160944123619972</v>
       </c>
       <c r="C29" t="n">
-        <v>1.164960843052714</v>
+        <v>1.160054983682173</v>
       </c>
       <c r="D29" t="n">
-        <v>1.166801188822903</v>
+        <v>1.161794238337976</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="3" t="n">
-        <v>45887.97916666666</v>
+      <c r="A30" s="2" t="n">
+        <v>45891.36111111111</v>
       </c>
       <c r="B30" t="n">
-        <v>1.16591267329054</v>
+        <v>1.160958574095763</v>
       </c>
       <c r="C30" t="n">
-        <v>1.165004841869653</v>
+        <v>1.160112115817471</v>
       </c>
       <c r="D30" t="n">
-        <v>1.166769730301765</v>
+        <v>1.161804366781888</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="n">
-        <v>45887.98263888889</v>
+      <c r="A31" s="2" t="n">
+        <v>45891.36458333334</v>
       </c>
       <c r="B31" t="n">
-        <v>1.165911042018876</v>
+        <v>1.160973383591289</v>
       </c>
       <c r="C31" t="n">
-        <v>1.165024747079715</v>
+        <v>1.160095912656926</v>
       </c>
       <c r="D31" t="n">
-        <v>1.166811529687462</v>
+        <v>1.161812979408142</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="n">
-        <v>45887.98611111111</v>
+      <c r="A32" s="2" t="n">
+        <v>45891.36805555555</v>
       </c>
       <c r="B32" t="n">
-        <v>1.165909811505237</v>
+        <v>1.160988552950585</v>
       </c>
       <c r="C32" t="n">
-        <v>1.164968876784187</v>
+        <v>1.1600911536666</v>
       </c>
       <c r="D32" t="n">
-        <v>1.166803618590016</v>
+        <v>1.161859166809596</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="n">
-        <v>45887.98958333334</v>
+      <c r="A33" s="2" t="n">
+        <v>45891.37152777778</v>
       </c>
       <c r="B33" t="n">
-        <v>1.165908983917058</v>
+        <v>1.161004082997092</v>
       </c>
       <c r="C33" t="n">
-        <v>1.165039228090216</v>
+        <v>1.160102686133122</v>
       </c>
       <c r="D33" t="n">
-        <v>1.166841453150235</v>
+        <v>1.161935270740246</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="3" t="n">
-        <v>45887.99305555555</v>
+      <c r="A34" s="2" t="n">
+        <v>45891.375</v>
       </c>
       <c r="B34" t="n">
-        <v>1.165908561395109</v>
+        <v>1.161019974533547</v>
       </c>
       <c r="C34" t="n">
-        <v>1.16496835222641</v>
+        <v>1.160145236768119</v>
       </c>
       <c r="D34" t="n">
-        <v>1.166817273813524</v>
+        <v>1.161945674868848</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="n">
-        <v>45887.99652777778</v>
+      <c r="A35" s="2" t="n">
+        <v>45891.37847222222</v>
       </c>
       <c r="B35" t="n">
-        <v>1.165908546053113</v>
+        <v>1.161036228341896</v>
       </c>
       <c r="C35" t="n">
-        <v>1.165007433633424</v>
+        <v>1.16010177366383</v>
       </c>
       <c r="D35" t="n">
-        <v>1.16680502193797</v>
+        <v>1.162013485265524</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="n">
-        <v>45888</v>
+      <c r="A36" s="2" t="n">
+        <v>45891.38194444445</v>
       </c>
       <c r="B36" t="n">
-        <v>1.165908939977675</v>
+        <v>1.161052845183202</v>
       </c>
       <c r="C36" t="n">
-        <v>1.165036813220352</v>
+        <v>1.160139059791908</v>
       </c>
       <c r="D36" t="n">
-        <v>1.166836513146237</v>
+        <v>1.161945475908698</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="3" t="n">
-        <v>45888.00347222222</v>
+      <c r="A37" s="2" t="n">
+        <v>45891.38541666666</v>
       </c>
       <c r="B37" t="n">
-        <v>1.165909745228063</v>
+        <v>1.161069825797653</v>
       </c>
       <c r="C37" t="n">
-        <v>1.164962394195723</v>
+        <v>1.160192867487304</v>
       </c>
       <c r="D37" t="n">
-        <v>1.166826117850115</v>
+        <v>1.161983303631443</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="n">
-        <v>45888.00694444445</v>
+      <c r="A38" s="2" t="n">
+        <v>45891.38888888889</v>
       </c>
       <c r="B38" t="n">
-        <v>1.1659109638361</v>
+        <v>1.161087170904332</v>
       </c>
       <c r="C38" t="n">
-        <v>1.16491321162177</v>
+        <v>1.160211643638605</v>
       </c>
       <c r="D38" t="n">
-        <v>1.16681880303222</v>
+        <v>1.162080384703046</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="n">
-        <v>45888.01041666666</v>
+      <c r="A39" s="2" t="n">
+        <v>45891.39236111111</v>
       </c>
       <c r="B39" t="n">
-        <v>1.165912597805971</v>
+        <v>1.161104881201197</v>
       </c>
       <c r="C39" t="n">
-        <v>1.164885420777068</v>
+        <v>1.160208046744355</v>
       </c>
       <c r="D39" t="n">
-        <v>1.166853407201025</v>
+        <v>1.162089694768189</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="n">
-        <v>45888.01388888889</v>
+      <c r="A40" s="2" t="n">
+        <v>45891.39583333334</v>
       </c>
       <c r="B40" t="n">
-        <v>1.165914649114028</v>
+        <v>1.161122957365114</v>
       </c>
       <c r="C40" t="n">
-        <v>1.164945827383602</v>
+        <v>1.160177325188597</v>
       </c>
       <c r="D40" t="n">
-        <v>1.16685508834651</v>
+        <v>1.162149654187374</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="n">
-        <v>45888.01736111111</v>
+      <c r="A41" s="2" t="n">
+        <v>45891.39930555555</v>
       </c>
       <c r="B41" t="n">
-        <v>1.165917119708739</v>
+        <v>1.161141400051606</v>
       </c>
       <c r="C41" t="n">
-        <v>1.164908754589213</v>
+        <v>1.160222916903312</v>
       </c>
       <c r="D41" t="n">
-        <v>1.166919034746204</v>
+        <v>1.16210118030845</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="3" t="n">
-        <v>45888.02083333334</v>
+      <c r="A42" s="2" t="n">
+        <v>45891.40277777778</v>
       </c>
       <c r="B42" t="n">
-        <v>1.165920011510298</v>
+        <v>1.161160209894828</v>
       </c>
       <c r="C42" t="n">
-        <v>1.164844817617458</v>
+        <v>1.160175799000632</v>
       </c>
       <c r="D42" t="n">
-        <v>1.166923337335377</v>
+        <v>1.162149227729061</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="3" t="n">
-        <v>45888.02430555555</v>
+      <c r="A43" s="2" t="n">
+        <v>45891.40625</v>
       </c>
       <c r="B43" t="n">
-        <v>1.16592332641085</v>
+        <v>1.161179387507572</v>
       </c>
       <c r="C43" t="n">
-        <v>1.164817507028278</v>
+        <v>1.160198667535964</v>
       </c>
       <c r="D43" t="n">
-        <v>1.166822013325274</v>
+        <v>1.162226949249886</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="n">
-        <v>45888.02777777778</v>
+      <c r="A44" s="2" t="n">
+        <v>45891.40972222222</v>
       </c>
       <c r="B44" t="n">
-        <v>1.165927066273962</v>
+        <v>1.161198933481145</v>
       </c>
       <c r="C44" t="n">
-        <v>1.164868449522612</v>
+        <v>1.160258425929091</v>
       </c>
       <c r="D44" t="n">
-        <v>1.166955949589592</v>
+        <v>1.162208121533136</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="n">
-        <v>45888.03125</v>
+      <c r="A45" s="2" t="n">
+        <v>45891.41319444445</v>
       </c>
       <c r="B45" t="n">
-        <v>1.165931232934661</v>
+        <v>1.161218848385242</v>
       </c>
       <c r="C45" t="n">
-        <v>1.164895602259762</v>
+        <v>1.1602189381283</v>
       </c>
       <c r="D45" t="n">
-        <v>1.1669055651678</v>
+        <v>1.162272141063583</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="3" t="n">
-        <v>45888.03472222222</v>
+      <c r="A46" s="2" t="n">
+        <v>45891.41666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>1.165935828199314</v>
+        <v>1.161239132767974</v>
       </c>
       <c r="C46" t="n">
-        <v>1.164761154757448</v>
+        <v>1.160252957139093</v>
       </c>
       <c r="D46" t="n">
-        <v>1.166943782601546</v>
+        <v>1.162298646276836</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="3" t="n">
-        <v>45888.03819444445</v>
+      <c r="A47" s="2" t="n">
+        <v>45891.42013888889</v>
       </c>
       <c r="B47" t="n">
-        <v>1.165940853845377</v>
+        <v>1.161259787155728</v>
       </c>
       <c r="C47" t="n">
-        <v>1.164867142812343</v>
+        <v>1.160239512862455</v>
       </c>
       <c r="D47" t="n">
-        <v>1.166949821656841</v>
+        <v>1.16227342610411</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="3" t="n">
-        <v>45888.04166666666</v>
+      <c r="A48" s="2" t="n">
+        <v>45891.42361111111</v>
       </c>
       <c r="B48" t="n">
-        <v>1.165946311621344</v>
+        <v>1.161280812053096</v>
       </c>
       <c r="C48" t="n">
-        <v>1.164859491295605</v>
+        <v>1.160281305941881</v>
       </c>
       <c r="D48" t="n">
-        <v>1.166969918332884</v>
+        <v>1.162298648830711</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="3" t="n">
-        <v>45888.04513888889</v>
+      <c r="A49" s="2" t="n">
+        <v>45891.42708333334</v>
       </c>
       <c r="B49" t="n">
-        <v>1.165952203246485</v>
+        <v>1.161302207942969</v>
       </c>
       <c r="C49" t="n">
-        <v>1.164887727412576</v>
+        <v>1.16021859494556</v>
       </c>
       <c r="D49" t="n">
-        <v>1.167025521093946</v>
+        <v>1.16242671493355</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="3" t="n">
-        <v>45888.04861111111</v>
+      <c r="A50" s="2" t="n">
+        <v>45891.43055555555</v>
       </c>
       <c r="B50" t="n">
-        <v>1.165958530410946</v>
+        <v>1.161323975286196</v>
       </c>
       <c r="C50" t="n">
-        <v>1.164922668541363</v>
+        <v>1.160279563425995</v>
       </c>
       <c r="D50" t="n">
-        <v>1.167026096808181</v>
+        <v>1.162397083106223</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="n">
-        <v>45888.05208333334</v>
+      <c r="A51" s="2" t="n">
+        <v>45891.43402777778</v>
       </c>
       <c r="B51" t="n">
-        <v>1.165965294775256</v>
+        <v>1.161346114521794</v>
       </c>
       <c r="C51" t="n">
-        <v>1.164777105662496</v>
+        <v>1.160313580454456</v>
       </c>
       <c r="D51" t="n">
-        <v>1.167042912342661</v>
+        <v>1.162429998863431</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>45891.4375</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1.161368626066716</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1.160283029955464</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1.162391177554488</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>45891.44097222222</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1.161391510315824</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1.160385830864833</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1.162568062197538</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>45891.44444444445</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1.161414767641928</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1.160416156447122</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1.162563305937806</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>45891.44791666666</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.161438398395573</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1.160361954452718</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1.162626552888589</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45891.45138888889</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.161462402905193</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1.160355620213861</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1.162636844949571</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>45891.45486111111</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1.161486781476835</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1.160372265793803</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1.162665202175061</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>45891.45833333334</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1.161511534394296</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1.16039075827283</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1.162838503164199</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45891.46180555555</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1.161536661918933</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1.160381372910557</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1.162849632256785</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>45891.46527777778</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1.161562164289774</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1.160342909707352</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1.162874623148744</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45891.46875</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1.161588041723305</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1.160281883151382</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1.162893241008126</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>45891.47222222222</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1.161614294413498</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1.160380191186078</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1.162941711205186</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>45891.47569444445</v>
+      </c>
+      <c r="B63" t="n">
+        <v>1.161640922531895</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1.160442700952257</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1.162986649795117</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>45891.47916666666</v>
+      </c>
+      <c r="B64" t="n">
+        <v>1.161667926227331</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1.160451074381211</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1.163058068845355</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="n">
+        <v>45891.48263888889</v>
+      </c>
+      <c r="B65" t="n">
+        <v>1.161695305626088</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1.160457866756223</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1.162955111221819</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>45891.48611111111</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.161723060831736</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1.160394518943331</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1.163138262944823</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>45891.48958333334</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1.161751191925266</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1.160330045502562</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1.163166814450034</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>45891.49305555555</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.161779698964828</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1.160410491266096</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1.163319787688039</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45891.49652777778</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.16180858198594</v>
+      </c>
+      <c r="C69" t="n">
+        <v>1.160421384104942</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1.163346857423076</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>45891.5</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.161837841001258</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1.160454180049541</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1.163295166595558</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>45891.50347222222</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.161867476000644</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1.160400973994018</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1.163572658294459</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45891.50694444445</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1.161897486951219</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1.160439900898288</v>
+      </c>
+      <c r="D72" t="n">
+        <v>1.163510558697092</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>45891.51041666666</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1.161927873797168</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1.160446290803184</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1.163757085450673</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>45891.51388888889</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1.161958636459805</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1.160377179159227</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1.163680208036361</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>45891.51736111111</v>
+      </c>
+      <c r="B75" t="n">
+        <v>1.161989774837626</v>
+      </c>
+      <c r="C75" t="n">
+        <v>1.160439625960069</v>
+      </c>
+      <c r="D75" t="n">
+        <v>1.1637269461852</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>45891.52083333334</v>
+      </c>
+      <c r="B76" t="n">
+        <v>1.162021288806217</v>
+      </c>
+      <c r="C76" t="n">
+        <v>1.160571227652276</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1.163794147894689</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>45891.52430555555</v>
+      </c>
+      <c r="B77" t="n">
+        <v>1.162053178218186</v>
+      </c>
+      <c r="C77" t="n">
+        <v>1.16058768086109</v>
+      </c>
+      <c r="D77" t="n">
+        <v>1.163727919758494</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>45891.52777777778</v>
+      </c>
+      <c r="B78" t="n">
+        <v>1.162085442903239</v>
+      </c>
+      <c r="C78" t="n">
+        <v>1.160478363199734</v>
+      </c>
+      <c r="D78" t="n">
+        <v>1.163948403768031</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>45891.53125</v>
+      </c>
+      <c r="B79" t="n">
+        <v>1.162118082668142</v>
+      </c>
+      <c r="C79" t="n">
+        <v>1.160442319942035</v>
+      </c>
+      <c r="D79" t="n">
+        <v>1.164089241645195</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>45891.53472222222</v>
+      </c>
+      <c r="B80" t="n">
+        <v>1.162151097296671</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1.160680304123268</v>
+      </c>
+      <c r="D80" t="n">
+        <v>1.164066908461089</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>45891.53819444445</v>
+      </c>
+      <c r="B81" t="n">
+        <v>1.162184486549736</v>
+      </c>
+      <c r="C81" t="n">
+        <v>1.160685995819022</v>
+      </c>
+      <c r="D81" t="n">
+        <v>1.164030983988822</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>45891.54166666666</v>
+      </c>
+      <c r="B82" t="n">
+        <v>1.162218250165185</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1.160625964180193</v>
+      </c>
+      <c r="D82" t="n">
+        <v>1.164198274987202</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>45891.54513888889</v>
+      </c>
+      <c r="B83" t="n">
+        <v>1.162252387857893</v>
+      </c>
+      <c r="C83" t="n">
+        <v>1.160459665680281</v>
+      </c>
+      <c r="D83" t="n">
+        <v>1.164526382282197</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45891.54861111111</v>
+      </c>
+      <c r="B84" t="n">
+        <v>1.162286899319824</v>
+      </c>
+      <c r="C84" t="n">
+        <v>1.160492154330695</v>
+      </c>
+      <c r="D84" t="n">
+        <v>1.1643647627621</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>45891.55208333334</v>
+      </c>
+      <c r="B85" t="n">
+        <v>1.162321784219966</v>
+      </c>
+      <c r="C85" t="n">
+        <v>1.160563965609989</v>
+      </c>
+      <c r="D85" t="n">
+        <v>1.164445895450265</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>45891.55555555555</v>
+      </c>
+      <c r="B86" t="n">
+        <v>1.162357042204232</v>
+      </c>
+      <c r="C86" t="n">
+        <v>1.160491347499027</v>
+      </c>
+      <c r="D86" t="n">
+        <v>1.16461175980949</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>45891.55902777778</v>
+      </c>
+      <c r="B87" t="n">
+        <v>1.162392672895697</v>
+      </c>
+      <c r="C87" t="n">
+        <v>1.160452501283769</v>
+      </c>
+      <c r="D87" t="n">
+        <v>1.164638569632292</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>45891.5625</v>
+      </c>
+      <c r="B88" t="n">
+        <v>1.162428675894366</v>
+      </c>
+      <c r="C88" t="n">
+        <v>1.160423781408477</v>
+      </c>
+      <c r="D88" t="n">
+        <v>1.164727809996347</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>45891.56597222222</v>
+      </c>
+      <c r="B89" t="n">
+        <v>1.162465050777317</v>
+      </c>
+      <c r="C89" t="n">
+        <v>1.160512387247993</v>
+      </c>
+      <c r="D89" t="n">
+        <v>1.164805027986283</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>45891.56944444445</v>
+      </c>
+      <c r="B90" t="n">
+        <v>1.162501797098672</v>
+      </c>
+      <c r="C90" t="n">
+        <v>1.16039661986884</v>
+      </c>
+      <c r="D90" t="n">
+        <v>1.164892687228916</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="n">
+        <v>45891.57291666666</v>
+      </c>
+      <c r="B91" t="n">
+        <v>1.162538914389576</v>
+      </c>
+      <c r="C91" t="n">
+        <v>1.160401351755087</v>
+      </c>
+      <c r="D91" t="n">
+        <v>1.165106128330596</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="n">
+        <v>45891.57638888889</v>
+      </c>
+      <c r="B92" t="n">
+        <v>1.162576402158346</v>
+      </c>
+      <c r="C92" t="n">
+        <v>1.160434589822771</v>
+      </c>
+      <c r="D92" t="n">
+        <v>1.165269442341743</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>45891.57986111111</v>
+      </c>
+      <c r="B93" t="n">
+        <v>1.162614259890238</v>
+      </c>
+      <c r="C93" t="n">
+        <v>1.160539167409014</v>
+      </c>
+      <c r="D93" t="n">
+        <v>1.165263594288902</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="n">
+        <v>45891.58333333334</v>
+      </c>
+      <c r="B94" t="n">
+        <v>1.162652487047714</v>
+      </c>
+      <c r="C94" t="n">
+        <v>1.160519959284701</v>
+      </c>
+      <c r="D94" t="n">
+        <v>1.165135207765704</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>45891.58680555555</v>
+      </c>
+      <c r="B95" t="n">
+        <v>1.162691083070347</v>
+      </c>
+      <c r="C95" t="n">
+        <v>1.160535959393074</v>
+      </c>
+      <c r="D95" t="n">
+        <v>1.165514026670866</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>45891.59027777778</v>
+      </c>
+      <c r="B96" t="n">
+        <v>1.162730047374772</v>
+      </c>
+      <c r="C96" t="n">
+        <v>1.160355377164749</v>
+      </c>
+      <c r="D96" t="n">
+        <v>1.165425336013157</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>45891.59375</v>
+      </c>
+      <c r="B97" t="n">
+        <v>1.162769379354811</v>
+      </c>
+      <c r="C97" t="n">
+        <v>1.160565255788114</v>
+      </c>
+      <c r="D97" t="n">
+        <v>1.165483415398886</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>45891.59722222222</v>
+      </c>
+      <c r="B98" t="n">
+        <v>1.162809078381424</v>
+      </c>
+      <c r="C98" t="n">
+        <v>1.16048063528643</v>
+      </c>
+      <c r="D98" t="n">
+        <v>1.16561113444921</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>45891.60069444445</v>
+      </c>
+      <c r="B99" t="n">
+        <v>1.162849143802888</v>
+      </c>
+      <c r="C99" t="n">
+        <v>1.16033996404014</v>
+      </c>
+      <c r="D99" t="n">
+        <v>1.165758987347971</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>45891.60416666666</v>
+      </c>
+      <c r="B100" t="n">
+        <v>1.162889574944585</v>
+      </c>
+      <c r="C100" t="n">
+        <v>1.160439993792725</v>
+      </c>
+      <c r="D100" t="n">
+        <v>1.165768317378061</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>45891.60763888889</v>
+      </c>
+      <c r="B101" t="n">
+        <v>1.162930371109194</v>
+      </c>
+      <c r="C101" t="n">
+        <v>1.160388224040774</v>
+      </c>
+      <c r="D101" t="n">
+        <v>1.165743317892503</v>
       </c>
     </row>
   </sheetData>
@@ -1209,17 +1906,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>mantener</t>
+          <t>comprar</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>199.63</v>
       </c>
       <c r="C2" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>45887.54703189815</v>
+      <c r="D2" s="2" t="n">
+        <v>45890.92865543389</v>
       </c>
     </row>
   </sheetData>
@@ -1266,18 +1963,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ninguna</t>
+          <t>compra</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>199.63</v>
       </c>
       <c r="C2" t="n">
-        <v>1.1665</v>
+        <v>1.16058</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sin acción</t>
+          <t>simulada</t>
         </is>
       </c>
     </row>
@@ -1329,287 +2026,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7e-06</v>
+        <v>4.1e-05</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.0035</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>mantener</t>
+          <t>comprar</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>199.63</v>
       </c>
       <c r="E2" t="n">
         <v>0.0005</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Simbolo</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Timeframe</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Modelo</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Pasos_pred</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>MAE</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>RMSE</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>MAPE_%</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>R2</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Sortino</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Accuracy_direccional</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Horizonte_dias</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Horizonte_horas_totales</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="n">
-        <v>45887.54705987268</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>EURUSD</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>M5</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>prophet</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>50</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.0003469403831574303</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.0004339600357957925</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.02973148080781424</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.4608994126733642</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-0.4013161612794071</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.5102040816326531</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>4.083333333333333</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Simbolo</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Timeframe</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Modelo</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Pasos_pred</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>MAE</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>RMSE</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>MAPE_%</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>R2</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Sortino</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Accuracy_direccional</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Horizonte_dias</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Horizonte_horas_totales</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="n">
-        <v>45887.5470598722</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>EURUSD</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>M5</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>prophet</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>50</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.0003469403831574303</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.0004339600357957925</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.02973148080781424</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.4608994126733642</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-0.4013161612794071</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.5102040816326531</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>4.083333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>